<commit_message>
Added easy collection solutions
</commit_message>
<xml_diff>
--- a/Leetcode-count.xlsx
+++ b/Leetcode-count.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -40,31 +40,37 @@
     <t xml:space="preserve">LinkedLists</t>
   </si>
   <si>
+    <t xml:space="preserve">Trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorting and Searching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EasySum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETA: 10 Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trees and Graphs</t>
   </si>
   <si>
     <t xml:space="preserve">BackTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorting and Searching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dynamic Programming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Math</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EasySum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium</t>
   </si>
   <si>
     <t xml:space="preserve">MediumSum</t>
@@ -91,6 +97,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -176,13 +183,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.09"/>
@@ -247,7 +254,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -258,7 +265,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -269,7 +276,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,7 +287,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,62 +298,65 @@
         <v>4</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="D10" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>6</v>
+      <c r="F10" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
+      <c r="A12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +367,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,7 +378,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -390,7 +400,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,62 +411,62 @@
         <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>5</v>
+      <c r="D21" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1"/>
+      <c r="A23" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,10 +474,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,10 +485,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -486,10 +496,10 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,10 +507,10 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,41 +518,30 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>4</v>
+      <c r="D32" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="0" t="n">
-        <f aca="false">SUM(C2:C32)</f>
+      <c r="D34" s="0" t="n">
+        <f aca="false">SUM(C2:C31)</f>
         <v>145</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>18</v>
+      <c r="E34" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added day 5 challenge
</commit_message>
<xml_diff>
--- a/Leetcode-count.xlsx
+++ b/Leetcode-count.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -31,37 +31,49 @@
     <t xml:space="preserve">No. of Problems</t>
   </si>
   <si>
+    <t xml:space="preserve">Remaining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days Spent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedLists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorting and Searching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EasySum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETA: 10 Days</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arrays and Strings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkedLists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorting and Searching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dynamic Programming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Math</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EasySum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETA: 10 Days</t>
   </si>
   <si>
     <t xml:space="preserve">Medium</t>
@@ -92,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -113,6 +125,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,8 +174,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,13 +204,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.09"/>
@@ -206,187 +227,202 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>2</v>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="0" t="n">
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>7</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>4</v>
@@ -394,157 +430,173 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="0" t="n">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1"/>
+      <c r="G22" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>6</v>
-      </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C31" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="0" t="n">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="1"/>
+      <c r="G33" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="0" t="n">
-        <f aca="false">SUM(C2:C31)</f>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="0" t="n">
+        <f aca="false">SUM(C2:C32)</f>
         <v>145</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>20</v>
+      <c r="G35" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E2:E10"/>
+    <mergeCell ref="E13:E21"/>
+    <mergeCell ref="E24:E32"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added tree traversals and more medium challenge solutions
</commit_message>
<xml_diff>
--- a/Leetcode-count.xlsx
+++ b/Leetcode-count.xlsx
@@ -180,10 +180,10 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.09"/>
@@ -397,7 +397,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,7 +453,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,7 +477,7 @@
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">SUM(D13:D21)</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G22" s="1"/>
     </row>

</xml_diff>